<commit_message>
curriculum change is dynamic,calendar details is done,curriculum change insertion is continuing
</commit_message>
<xml_diff>
--- a/phpexcel/excelfiles/FACExcel2.xlsx
+++ b/phpexcel/excelfiles/FACExcel2.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>First Name</t>
   </si>
@@ -89,9 +89,6 @@
   </si>
   <si>
     <t>Freshman</t>
-  </si>
-  <si>
-    <t>lorem</t>
   </si>
   <si>
     <t>Balkh</t>
@@ -573,13 +570,13 @@
         <v>11</v>
       </c>
       <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
         <v>24</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>25</v>
-      </c>
-      <c r="O2" t="s">
-        <v>26</v>
       </c>
       <c r="P2" t="s">
         <v>15</v>
@@ -626,10 +623,10 @@
         <v>5</v>
       </c>
       <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
         <v>27</v>
-      </c>
-      <c r="H3" t="s">
-        <v>28</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -644,10 +641,10 @@
         <v>11</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="O3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P3" t="s">
         <v>15</v>
@@ -821,10 +818,10 @@
         <v>5</v>
       </c>
       <c r="G2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
         <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>31</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -839,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="O2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="P2" t="s">
         <v>15</v>

</xml_diff>